<commit_message>
Ajustes na função de enviar email, no README.md e no arquivo principal main.py
</commit_message>
<xml_diff>
--- a/imoveis_filtrados.xlsx
+++ b/imoveis_filtrados.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,418 +440,598 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>numero_imovel</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>uf</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>cidade</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>bairro</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>preco</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>valor_avaliacao</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>desconto</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>modalidade_venda</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>imovel</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>metro_quadrado_m3</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>metro_quadrado_area_total_m3</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>link_acesso</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>data_processamento</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>10137825</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">CARANGOLA </t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t xml:space="preserve">RESID. SANTA MARIA </t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>22233.99</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>48000</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>53.68</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Venda Online</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
         <v>0</v>
       </c>
-      <c r="H2" t="n">
+      <c r="K2" t="n">
         <v>21832</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>https://venda-imoveis.caixa.gov.br/sistema/detalhe-imovel.asp?hdnOrigem=index&amp;hdnimovel=10137825</t>
         </is>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>45673.75602836806</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>10137826</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">CARANGOLA </t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t xml:space="preserve">RESID. SANTA MARIA </t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>22233.99</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>48000</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>53.68</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Venda Online</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="n">
+      <c r="K3" t="n">
         <v>21893</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>https://venda-imoveis.caixa.gov.br/sistema/detalhe-imovel.asp?hdnOrigem=index&amp;hdnimovel=10137826</t>
         </is>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>45673.75602836806</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>10137827</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">CARANGOLA </t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t xml:space="preserve">RESID. SANTA MARIA </t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>22233.99</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>48000</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>53.68</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Venda Online</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
         <v>0</v>
       </c>
-      <c r="H4" t="n">
+      <c r="K4" t="n">
         <v>21954</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>https://venda-imoveis.caixa.gov.br/sistema/detalhe-imovel.asp?hdnOrigem=index&amp;hdnimovel=10137827</t>
         </is>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>45673.75602836806</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>1444407695527</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">FERVEDOURO </t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t xml:space="preserve">LOT MARTINS DO PRADO </t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>22476.89</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>45000</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>50.06</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Venda Direta Online</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" t="n">
+      <c r="K5" t="n">
         <v>15000</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>https://venda-imoveis.caixa.gov.br/sistema/detalhe-imovel.asp?hdnOrigem=index&amp;hdnimovel=1444407695527</t>
         </is>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>45673.75602836806</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>10137828</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">CARANGOLA </t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t xml:space="preserve">RESID. SANTA MARIA </t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>24086.82</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>52000</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>53.68</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Venda Online</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
         <v>0</v>
       </c>
-      <c r="H6" t="n">
+      <c r="K6" t="n">
         <v>24249</v>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>https://venda-imoveis.caixa.gov.br/sistema/detalhe-imovel.asp?hdnOrigem=index&amp;hdnimovel=10137828</t>
         </is>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>45673.75602836806</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>10171235</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">MURIAE </t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t xml:space="preserve">GASPAR </t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>24405.51</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>44037.72</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>44.59</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Venda Direta Online</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
         <v>0</v>
       </c>
-      <c r="H7" t="n">
+      <c r="K7" t="n">
         <v>16000</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>https://venda-imoveis.caixa.gov.br/sistema/detalhe-imovel.asp?hdnOrigem=index&amp;hdnimovel=10171235</t>
         </is>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>45673.75602836806</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>10153991</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">SAO BRAS DO SUACUI </t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t xml:space="preserve">MASTERVILLE II </t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>25118.91</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>49000</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>48.74</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Venda Online</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
         <v>0</v>
       </c>
-      <c r="H8" t="n">
+      <c r="K8" t="n">
         <v>25761</v>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>https://venda-imoveis.caixa.gov.br/sistema/detalhe-imovel.asp?hdnOrigem=index&amp;hdnimovel=10153991</t>
         </is>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>45673.75602836806</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>8444409794539</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve">PASSOS </t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t xml:space="preserve">ACLIMACAO </t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>25631.54</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>50000</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>48.74</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Venda Direta Online</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
         <v>6996</v>
       </c>
-      <c r="H9" t="n">
+      <c r="K9" t="n">
         <v>12500</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>https://venda-imoveis.caixa.gov.br/sistema/detalhe-imovel.asp?hdnOrigem=index&amp;hdnimovel=8444409794539</t>
         </is>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>45673.75602836806</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="n">
+        <v>10137830</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve">CARANGOLA </t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t xml:space="preserve">RESID. SANTA MARIA </t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>26402.86</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>57000</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>53.68</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Venda Online</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
         <v>0</v>
       </c>
-      <c r="H10" t="n">
+      <c r="K10" t="n">
         <v>28098</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>https://venda-imoveis.caixa.gov.br/sistema/detalhe-imovel.asp?hdnOrigem=index&amp;hdnimovel=10137830</t>
         </is>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>45673.75602836806</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="n">
+        <v>10153988</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve">SAO BRAS DO SUACUI </t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t xml:space="preserve">MASTERVILLE II </t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>28707.32</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>56000</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>48.74</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Venda Online</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Terreno</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
         <v>0</v>
       </c>
-      <c r="H11" t="n">
+      <c r="K11" t="n">
         <v>29834</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>https://venda-imoveis.caixa.gov.br/sistema/detalhe-imovel.asp?hdnOrigem=index&amp;hdnimovel=10153988</t>
         </is>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>45673.75602836806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>